<commit_message>
create entry module completed..
</commit_message>
<xml_diff>
--- a/Documentation/statamic taskslist.xlsx
+++ b/Documentation/statamic taskslist.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/statamic/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7CBB1B0-5D4C-0747-B5C9-993376823543}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D62A7906-AFFA-1B48-9776-AE459B42702E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="500" windowWidth="38400" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="155">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -479,18 +479,34 @@
   </si>
   <si>
     <t>/login, /register</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Create Users Model</t>
+  </si>
+  <si>
+    <t>Set up routes for users</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -680,15 +696,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -697,49 +710,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -748,16 +752,31 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1039,485 +1058,521 @@
   <dimension ref="A1:G204"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="111" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="H126" sqref="H126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.83203125" style="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.83203125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="35.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.83203125" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.83203125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
     </row>
     <row r="2" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
     </row>
     <row r="3" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="12"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="25"/>
     </row>
     <row r="5" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="13">
+      <c r="A5" s="9">
         <v>1</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="16"/>
+      <c r="C5" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="6" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="17">
+      <c r="A6" s="13">
         <v>2</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="20"/>
+      <c r="F6" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="7" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="17">
+      <c r="A7" s="13">
         <v>3</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="20"/>
+      <c r="D7" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="8" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="13">
+      <c r="A8" s="9">
         <v>4</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="19" t="s">
+      <c r="C8" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" s="20"/>
+      <c r="D8" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="17">
+      <c r="A9" s="13">
         <v>5</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D9" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" s="20"/>
+      <c r="E9" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="10" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="17">
+      <c r="A10" s="13">
         <v>6</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10" s="20"/>
+      <c r="C10" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="11" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="13">
+      <c r="A11" s="9">
         <v>7</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F11" s="20"/>
+      <c r="C11" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="12" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="17">
+      <c r="A12" s="13">
         <v>8</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F12" s="20"/>
-      <c r="G12" s="26"/>
+      <c r="C12" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="G12" s="22"/>
     </row>
     <row r="13" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="17">
+      <c r="A13" s="13">
         <v>9</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F13" s="20"/>
+      <c r="C13" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="14" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="13">
+      <c r="A14" s="9">
         <v>10</v>
       </c>
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="E14" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F14" s="20"/>
+      <c r="C14" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="16"/>
     </row>
     <row r="15" spans="1:7" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="12"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="25"/>
     </row>
     <row r="16" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="13">
+      <c r="A16" s="9">
         <v>1</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" s="15" t="s">
+      <c r="C16" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="15" t="s">
+      <c r="E16" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="F16" s="16"/>
+      <c r="F16" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="17" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="17">
+      <c r="A17" s="13">
         <v>2</v>
       </c>
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="19" t="s">
+      <c r="C17" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="D17" s="15" t="s">
+      <c r="D17" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="E17" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F17" s="20"/>
+      <c r="E17" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="18" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="13">
+      <c r="A18" s="9">
         <v>3</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="19" t="s">
+      <c r="C18" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="15" t="s">
+      <c r="D18" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="E18" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F18" s="20"/>
+      <c r="E18" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="19" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="17">
+      <c r="A19" s="13">
         <v>4</v>
       </c>
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="19" t="s">
+      <c r="C19" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="D19" s="15" t="s">
+      <c r="D19" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="E19" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F19" s="20"/>
+      <c r="E19" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="20" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="13">
+      <c r="A20" s="9">
         <v>5</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="19" t="s">
+      <c r="C20" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="D20" s="15" t="s">
+      <c r="D20" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="E20" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F20" s="20"/>
+      <c r="E20" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="21" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="17">
+      <c r="A21" s="13">
         <v>6</v>
       </c>
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C21" s="19" t="s">
+      <c r="C21" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="D21" s="15" t="s">
+      <c r="D21" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="E21" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F21" s="20"/>
+      <c r="E21" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="22" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="13">
+      <c r="A22" s="9">
         <v>7</v>
       </c>
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="C22" s="19" t="s">
+      <c r="C22" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D22" s="15" t="s">
+      <c r="D22" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="E22" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F22" s="20"/>
+      <c r="E22" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F22" s="16"/>
     </row>
     <row r="23" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="17">
+      <c r="A23" s="13">
         <v>8</v>
       </c>
-      <c r="B23" s="18" t="s">
+      <c r="B23" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="19" t="s">
+      <c r="C23" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="D23" s="15" t="s">
+      <c r="D23" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="E23" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F23" s="20"/>
+      <c r="E23" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F23" s="16"/>
     </row>
     <row r="24" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="13">
+      <c r="A24" s="9">
         <v>9</v>
       </c>
-      <c r="B24" s="18" t="s">
+      <c r="B24" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C24" s="19" t="s">
+      <c r="C24" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="D24" s="15" t="s">
+      <c r="D24" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F24" s="20"/>
+      <c r="E24" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F24" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="25" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="17">
+      <c r="A25" s="13">
         <v>10</v>
       </c>
-      <c r="B25" s="18" t="s">
+      <c r="B25" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="D25" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="E25" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F25" s="20"/>
+      <c r="C25" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="26" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="13">
+      <c r="A26" s="9">
         <v>11</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C26" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="D26" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="E26" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F26" s="2"/>
+      <c r="C26" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E26" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="27" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="17">
+      <c r="A27" s="13">
         <v>12</v>
       </c>
-      <c r="B27" s="23" t="s">
+      <c r="B27" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="D27" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="E27" s="19" t="s">
+      <c r="C27" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E27" s="15" t="s">
         <v>19</v>
       </c>
       <c r="F27" s="2"/>
     </row>
     <row r="28" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="10" t="s">
+      <c r="A28" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="B28" s="11"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="12"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="25"/>
     </row>
     <row r="29" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
@@ -1526,16 +1581,18 @@
       <c r="B29" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C29" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="D29" s="24" t="s">
+      <c r="C29" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D29" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="E29" s="24" t="s">
+      <c r="E29" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="F29" s="2"/>
+      <c r="F29" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="30" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
@@ -1544,16 +1601,18 @@
       <c r="B30" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C30" s="21" t="s">
+      <c r="C30" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="D30" s="24" t="s">
+      <c r="D30" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="E30" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F30" s="2"/>
+      <c r="E30" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F30" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="31" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
@@ -1562,16 +1621,18 @@
       <c r="B31" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C31" s="21" t="s">
+      <c r="C31" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="D31" s="24" t="s">
+      <c r="D31" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="E31" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F31" s="2"/>
+      <c r="E31" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F31" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="32" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
@@ -1580,16 +1641,18 @@
       <c r="B32" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C32" s="21" t="s">
+      <c r="C32" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="D32" s="24" t="s">
+      <c r="D32" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="E32" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F32" s="2"/>
+      <c r="E32" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F32" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="33" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
@@ -1598,16 +1661,18 @@
       <c r="B33" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C33" s="21" t="s">
+      <c r="C33" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="D33" s="24" t="s">
+      <c r="D33" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="E33" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F33" s="2"/>
+      <c r="E33" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F33" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="34" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
@@ -1616,16 +1681,18 @@
       <c r="B34" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C34" s="21" t="s">
+      <c r="C34" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="D34" s="24" t="s">
+      <c r="D34" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="E34" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F34" s="2"/>
+      <c r="E34" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F34" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="35" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
@@ -1634,16 +1701,18 @@
       <c r="B35" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C35" s="21" t="s">
+      <c r="C35" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="D35" s="24" t="s">
+      <c r="D35" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="E35" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F35" s="2"/>
+      <c r="E35" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F35" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="36" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
@@ -1652,16 +1721,18 @@
       <c r="B36" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C36" s="21" t="s">
+      <c r="C36" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="D36" s="24" t="s">
+      <c r="D36" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="E36" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F36" s="2"/>
+      <c r="E36" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F36" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="37" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
@@ -1670,16 +1741,18 @@
       <c r="B37" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C37" s="21" t="s">
+      <c r="C37" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="D37" s="24" t="s">
+      <c r="D37" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="E37" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F37" s="2"/>
+      <c r="E37" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F37" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="38" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
@@ -1688,34 +1761,38 @@
       <c r="B38" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C38" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="D38" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="E38" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F38" s="2"/>
+      <c r="C38" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D38" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E38" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F38" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="39" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>11</v>
       </c>
-      <c r="B39" s="23" t="s">
+      <c r="B39" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="C39" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="D39" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="E39" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F39" s="2"/>
+      <c r="C39" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D39" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E39" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F39" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="40" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
@@ -1724,62 +1801,66 @@
       <c r="B40" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C40" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="D40" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="E40" s="19" t="s">
+      <c r="C40" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D40" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E40" s="15" t="s">
         <v>19</v>
       </c>
       <c r="F40" s="2"/>
     </row>
     <row r="41" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="10" t="s">
+      <c r="A41" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="B41" s="11"/>
-      <c r="C41" s="11"/>
-      <c r="D41" s="11"/>
-      <c r="E41" s="11"/>
-      <c r="F41" s="12"/>
+      <c r="B41" s="24"/>
+      <c r="C41" s="24"/>
+      <c r="D41" s="24"/>
+      <c r="E41" s="24"/>
+      <c r="F41" s="25"/>
     </row>
     <row r="42" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>1</v>
       </c>
-      <c r="B42" s="23" t="s">
+      <c r="B42" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="C42" s="19" t="s">
+      <c r="C42" s="15" t="s">
         <v>19</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E42" s="24" t="s">
+      <c r="E42" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="F42" s="6"/>
+      <c r="F42" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="43" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>2</v>
       </c>
-      <c r="B43" s="23" t="s">
+      <c r="B43" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="C43" s="21" t="s">
+      <c r="C43" s="17" t="s">
         <v>148</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E43" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F43" s="2"/>
+      <c r="E43" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F43" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="44" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
@@ -1788,16 +1869,18 @@
       <c r="B44" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C44" s="21" t="s">
+      <c r="C44" s="17" t="s">
         <v>148</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E44" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F44" s="6"/>
+      <c r="E44" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F44" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="45" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
@@ -1806,16 +1889,18 @@
       <c r="B45" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C45" s="21" t="s">
+      <c r="C45" s="17" t="s">
         <v>147</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E45" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F45" s="2"/>
+      <c r="E45" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F45" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="46" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
@@ -1824,16 +1909,18 @@
       <c r="B46" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C46" s="21" t="s">
+      <c r="C46" s="17" t="s">
         <v>146</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E46" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F46" s="2"/>
+      <c r="E46" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F46" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="47" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
@@ -1842,16 +1929,18 @@
       <c r="B47" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C47" s="21" t="s">
+      <c r="C47" s="17" t="s">
         <v>145</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E47" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F47" s="2"/>
+      <c r="E47" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F47" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="48" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
@@ -1860,16 +1949,18 @@
       <c r="B48" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C48" s="21" t="s">
+      <c r="C48" s="17" t="s">
         <v>144</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E48" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F48" s="2"/>
+      <c r="E48" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F48" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="49" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
@@ -1878,16 +1969,16 @@
       <c r="B49" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C49" s="25" t="s">
+      <c r="C49" s="21" t="s">
         <v>143</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E49" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F49" s="6"/>
+      <c r="E49" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F49" s="5"/>
     </row>
     <row r="50" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
@@ -1896,34 +1987,38 @@
       <c r="B50" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C50" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="D50" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="E50" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F50" s="6"/>
+      <c r="C50" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D50" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E50" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F50" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="51" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>10</v>
       </c>
-      <c r="B51" s="23" t="s">
+      <c r="B51" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="C51" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="D51" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="E51" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F51" s="6"/>
+      <c r="C51" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D51" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E51" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F51" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="52" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
@@ -1932,62 +2027,66 @@
       <c r="B52" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C52" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="D52" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="E52" s="19" t="s">
+      <c r="C52" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D52" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E52" s="15" t="s">
         <v>19</v>
       </c>
       <c r="F52" s="2"/>
     </row>
     <row r="53" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="10" t="s">
+      <c r="A53" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="B53" s="11"/>
-      <c r="C53" s="11"/>
-      <c r="D53" s="11"/>
-      <c r="E53" s="11"/>
-      <c r="F53" s="12"/>
+      <c r="B53" s="24"/>
+      <c r="C53" s="24"/>
+      <c r="D53" s="24"/>
+      <c r="E53" s="24"/>
+      <c r="F53" s="25"/>
     </row>
     <row r="54" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>1</v>
       </c>
-      <c r="B54" s="23" t="s">
+      <c r="B54" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="C54" s="19" t="s">
+      <c r="C54" s="15" t="s">
         <v>19</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E54" s="24" t="s">
+      <c r="E54" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="F54" s="2"/>
+      <c r="F54" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="55" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>2</v>
       </c>
-      <c r="B55" s="23" t="s">
+      <c r="B55" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="C55" s="21" t="s">
+      <c r="C55" s="17" t="s">
         <v>142</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E55" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F55" s="6"/>
+      <c r="E55" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F55" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="56" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
@@ -1996,16 +2095,18 @@
       <c r="B56" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C56" s="21" t="s">
+      <c r="C56" s="17" t="s">
         <v>142</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E56" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F56" s="6"/>
+      <c r="E56" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F56" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="57" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
@@ -2014,16 +2115,18 @@
       <c r="B57" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C57" s="21" t="s">
+      <c r="C57" s="17" t="s">
         <v>141</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E57" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F57" s="2"/>
+      <c r="E57" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F57" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="58" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
@@ -2032,16 +2135,18 @@
       <c r="B58" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C58" s="21" t="s">
+      <c r="C58" s="17" t="s">
         <v>140</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E58" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F58" s="2"/>
+      <c r="E58" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F58" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="59" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
@@ -2050,16 +2155,18 @@
       <c r="B59" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C59" s="21" t="s">
+      <c r="C59" s="17" t="s">
         <v>139</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E59" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F59" s="2"/>
+      <c r="E59" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F59" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="60" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
@@ -2068,16 +2175,18 @@
       <c r="B60" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C60" s="21" t="s">
+      <c r="C60" s="17" t="s">
         <v>138</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E60" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F60" s="6"/>
+      <c r="E60" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F60" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="61" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
@@ -2086,16 +2195,18 @@
       <c r="B61" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C61" s="21" t="s">
+      <c r="C61" s="17" t="s">
         <v>137</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E61" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F61" s="6"/>
+      <c r="E61" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F61" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="62" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
@@ -2104,13 +2215,13 @@
       <c r="B62" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C62" s="19" t="s">
+      <c r="C62" s="15" t="s">
         <v>19</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E62" s="19" t="s">
+      <c r="E62" s="15" t="s">
         <v>19</v>
       </c>
       <c r="F62" s="2"/>
@@ -2122,34 +2233,38 @@
       <c r="B63" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C63" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="D63" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="E63" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F63" s="6"/>
+      <c r="C63" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D63" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E63" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F63" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="64" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
         <v>11</v>
       </c>
-      <c r="B64" s="23" t="s">
+      <c r="B64" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="C64" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="D64" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="E64" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F64" s="2"/>
+      <c r="C64" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D64" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E64" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F64" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="65" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
@@ -2158,62 +2273,66 @@
       <c r="B65" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C65" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="D65" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="E65" s="19" t="s">
+      <c r="C65" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D65" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E65" s="15" t="s">
         <v>19</v>
       </c>
       <c r="F65" s="2"/>
     </row>
     <row r="66" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="10" t="s">
+      <c r="A66" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="B66" s="11"/>
-      <c r="C66" s="11"/>
-      <c r="D66" s="11"/>
-      <c r="E66" s="11"/>
-      <c r="F66" s="12"/>
+      <c r="B66" s="24"/>
+      <c r="C66" s="24"/>
+      <c r="D66" s="24"/>
+      <c r="E66" s="24"/>
+      <c r="F66" s="25"/>
     </row>
     <row r="67" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
         <v>1</v>
       </c>
-      <c r="B67" s="23" t="s">
+      <c r="B67" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="C67" s="19" t="s">
+      <c r="C67" s="15" t="s">
         <v>19</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E67" s="24" t="s">
+      <c r="E67" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="F67" s="2"/>
+      <c r="F67" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="68" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
         <v>2</v>
       </c>
-      <c r="B68" s="23" t="s">
+      <c r="B68" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="C68" s="21" t="s">
+      <c r="C68" s="17" t="s">
         <v>136</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E68" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F68" s="6"/>
+      <c r="E68" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F68" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="69" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
@@ -2222,16 +2341,18 @@
       <c r="B69" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C69" s="21" t="s">
+      <c r="C69" s="17" t="s">
         <v>136</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E69" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F69" s="2"/>
+      <c r="E69" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F69" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="70" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
@@ -2240,16 +2361,18 @@
       <c r="B70" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C70" s="21" t="s">
+      <c r="C70" s="17" t="s">
         <v>135</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E70" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F70" s="6"/>
+      <c r="E70" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F70" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="71" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="2">
@@ -2258,16 +2381,18 @@
       <c r="B71" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C71" s="21" t="s">
+      <c r="C71" s="17" t="s">
         <v>134</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E71" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F71" s="6"/>
+      <c r="E71" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F71" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="72" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
@@ -2276,16 +2401,18 @@
       <c r="B72" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C72" s="21" t="s">
+      <c r="C72" s="17" t="s">
         <v>133</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E72" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F72" s="2"/>
+      <c r="E72" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F72" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="73" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="2">
@@ -2294,16 +2421,18 @@
       <c r="B73" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C73" s="21" t="s">
+      <c r="C73" s="17" t="s">
         <v>132</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E73" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F73" s="2"/>
+      <c r="E73" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F73" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="74" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
@@ -2312,13 +2441,13 @@
       <c r="B74" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C74" s="21" t="s">
+      <c r="C74" s="17" t="s">
         <v>131</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E74" s="19" t="s">
+      <c r="E74" s="15" t="s">
         <v>19</v>
       </c>
       <c r="F74" s="2"/>
@@ -2330,34 +2459,38 @@
       <c r="B75" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C75" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="D75" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="E75" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F75" s="2"/>
+      <c r="C75" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D75" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E75" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F75" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="76" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="2">
         <v>10</v>
       </c>
-      <c r="B76" s="23" t="s">
+      <c r="B76" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="C76" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="D76" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="E76" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F76" s="6"/>
+      <c r="C76" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D76" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E76" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F76" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="77" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="2">
@@ -2366,62 +2499,66 @@
       <c r="B77" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C77" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="D77" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="E77" s="19" t="s">
+      <c r="C77" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D77" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E77" s="15" t="s">
         <v>19</v>
       </c>
       <c r="F77" s="2"/>
     </row>
     <row r="78" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="10" t="s">
+      <c r="A78" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="B78" s="11"/>
-      <c r="C78" s="11"/>
-      <c r="D78" s="11"/>
-      <c r="E78" s="11"/>
-      <c r="F78" s="12"/>
+      <c r="B78" s="24"/>
+      <c r="C78" s="24"/>
+      <c r="D78" s="24"/>
+      <c r="E78" s="24"/>
+      <c r="F78" s="25"/>
     </row>
     <row r="79" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="2">
         <v>1</v>
       </c>
-      <c r="B79" s="23" t="s">
+      <c r="B79" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="C79" s="19" t="s">
+      <c r="C79" s="15" t="s">
         <v>19</v>
       </c>
       <c r="D79" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="E79" s="24" t="s">
+      <c r="E79" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="F79" s="2"/>
+      <c r="F79" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="80" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="2">
         <v>2</v>
       </c>
-      <c r="B80" s="23" t="s">
+      <c r="B80" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="C80" s="21" t="s">
+      <c r="C80" s="17" t="s">
         <v>130</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="E80" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F80" s="2"/>
+      <c r="E80" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F80" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="81" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="2">
@@ -2430,16 +2567,18 @@
       <c r="B81" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C81" s="21" t="s">
+      <c r="C81" s="17" t="s">
         <v>130</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="E81" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F81" s="6"/>
+      <c r="E81" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F81" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="82" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="2">
@@ -2448,16 +2587,16 @@
       <c r="B82" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C82" s="21" t="s">
+      <c r="C82" s="17" t="s">
         <v>129</v>
       </c>
       <c r="D82" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="E82" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F82" s="6"/>
+      <c r="E82" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F82" s="5"/>
     </row>
     <row r="83" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="2">
@@ -2466,13 +2605,13 @@
       <c r="B83" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C83" s="21" t="s">
+      <c r="C83" s="17" t="s">
         <v>128</v>
       </c>
       <c r="D83" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="E83" s="19" t="s">
+      <c r="E83" s="15" t="s">
         <v>19</v>
       </c>
       <c r="F83" s="2"/>
@@ -2484,13 +2623,13 @@
       <c r="B84" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C84" s="21" t="s">
+      <c r="C84" s="17" t="s">
         <v>127</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="E84" s="19" t="s">
+      <c r="E84" s="15" t="s">
         <v>19</v>
       </c>
       <c r="F84" s="2"/>
@@ -2502,13 +2641,13 @@
       <c r="B85" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C85" s="21" t="s">
+      <c r="C85" s="17" t="s">
         <v>126</v>
       </c>
       <c r="D85" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="E85" s="19" t="s">
+      <c r="E85" s="15" t="s">
         <v>19</v>
       </c>
       <c r="F85" s="2"/>
@@ -2520,13 +2659,13 @@
       <c r="B86" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C86" s="21" t="s">
+      <c r="C86" s="17" t="s">
         <v>125</v>
       </c>
       <c r="D86" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="E86" s="19" t="s">
+      <c r="E86" s="15" t="s">
         <v>19</v>
       </c>
       <c r="F86" s="2"/>
@@ -2538,34 +2677,34 @@
       <c r="B87" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C87" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="D87" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="E87" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F87" s="6"/>
+      <c r="C87" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D87" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E87" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F87" s="5"/>
     </row>
     <row r="88" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="2">
         <v>10</v>
       </c>
-      <c r="B88" s="23" t="s">
+      <c r="B88" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="C88" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="D88" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="E88" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F88" s="6"/>
+      <c r="C88" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D88" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E88" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F88" s="5"/>
     </row>
     <row r="89" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="2">
@@ -2574,26 +2713,26 @@
       <c r="B89" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C89" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="D89" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="E89" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F89" s="6"/>
+      <c r="C89" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D89" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E89" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F89" s="5"/>
     </row>
     <row r="90" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="10" t="s">
+      <c r="A90" s="23" t="s">
         <v>118</v>
       </c>
-      <c r="B90" s="11"/>
-      <c r="C90" s="11"/>
-      <c r="D90" s="11"/>
-      <c r="E90" s="11"/>
-      <c r="F90" s="12"/>
+      <c r="B90" s="24"/>
+      <c r="C90" s="24"/>
+      <c r="D90" s="24"/>
+      <c r="E90" s="24"/>
+      <c r="F90" s="25"/>
     </row>
     <row r="91" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="2">
@@ -2602,16 +2741,18 @@
       <c r="B91" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C91" s="19" t="s">
+      <c r="C91" s="15" t="s">
         <v>19</v>
       </c>
       <c r="D91" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="E91" s="24" t="s">
+      <c r="E91" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="F91" s="2"/>
+      <c r="F91" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="92" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="2">
@@ -2620,16 +2761,18 @@
       <c r="B92" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C92" s="21" t="s">
+      <c r="C92" s="17" t="s">
         <v>124</v>
       </c>
       <c r="D92" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="E92" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F92" s="2"/>
+      <c r="E92" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F92" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="93" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="2">
@@ -2638,16 +2781,18 @@
       <c r="B93" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C93" s="21" t="s">
+      <c r="C93" s="17" t="s">
         <v>124</v>
       </c>
       <c r="D93" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="E93" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F93" s="6"/>
+      <c r="E93" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F93" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="94" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="2">
@@ -2656,16 +2801,18 @@
       <c r="B94" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C94" s="21" t="s">
+      <c r="C94" s="17" t="s">
         <v>123</v>
       </c>
       <c r="D94" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="E94" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F94" s="6"/>
+      <c r="E94" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F94" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="95" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="2">
@@ -2674,13 +2821,13 @@
       <c r="B95" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C95" s="21" t="s">
+      <c r="C95" s="17" t="s">
         <v>122</v>
       </c>
       <c r="D95" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="E95" s="19" t="s">
+      <c r="E95" s="15" t="s">
         <v>19</v>
       </c>
       <c r="F95" s="2"/>
@@ -2692,13 +2839,13 @@
       <c r="B96" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C96" s="21" t="s">
+      <c r="C96" s="17" t="s">
         <v>121</v>
       </c>
       <c r="D96" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="E96" s="19" t="s">
+      <c r="E96" s="15" t="s">
         <v>19</v>
       </c>
       <c r="F96" s="2"/>
@@ -2710,16 +2857,16 @@
       <c r="B97" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C97" s="21" t="s">
+      <c r="C97" s="17" t="s">
         <v>120</v>
       </c>
       <c r="D97" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="E97" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F97" s="6"/>
+      <c r="E97" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F97" s="5"/>
     </row>
     <row r="98" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="2">
@@ -2728,13 +2875,13 @@
       <c r="B98" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C98" s="21" t="s">
+      <c r="C98" s="17" t="s">
         <v>119</v>
       </c>
       <c r="D98" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="E98" s="19" t="s">
+      <c r="E98" s="15" t="s">
         <v>19</v>
       </c>
       <c r="F98" s="2"/>
@@ -2746,31 +2893,31 @@
       <c r="B99" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C99" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="D99" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="E99" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F99" s="6"/>
+      <c r="C99" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D99" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E99" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F99" s="5"/>
     </row>
     <row r="100" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="2">
         <v>10</v>
       </c>
-      <c r="B100" s="23" t="s">
+      <c r="B100" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="C100" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="D100" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="E100" s="19" t="s">
+      <c r="C100" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D100" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E100" s="15" t="s">
         <v>19</v>
       </c>
       <c r="F100" s="2"/>
@@ -2782,62 +2929,66 @@
       <c r="B101" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C101" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="D101" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="E101" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F101" s="6"/>
+      <c r="C101" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D101" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E101" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F101" s="5"/>
     </row>
     <row r="102" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="10" t="s">
+      <c r="A102" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="B102" s="11"/>
-      <c r="C102" s="11"/>
-      <c r="D102" s="11"/>
-      <c r="E102" s="11"/>
-      <c r="F102" s="12"/>
+      <c r="B102" s="24"/>
+      <c r="C102" s="24"/>
+      <c r="D102" s="24"/>
+      <c r="E102" s="24"/>
+      <c r="F102" s="25"/>
     </row>
     <row r="103" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="2">
         <v>1</v>
       </c>
-      <c r="B103" s="23" t="s">
+      <c r="B103" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="C103" s="19" t="s">
+      <c r="C103" s="15" t="s">
         <v>19</v>
       </c>
       <c r="D103" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="E103" s="24" t="s">
+      <c r="E103" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="F103" s="2"/>
+      <c r="F103" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="104" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="2">
         <v>2</v>
       </c>
-      <c r="B104" s="23" t="s">
+      <c r="B104" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="C104" s="21" t="s">
+      <c r="C104" s="17" t="s">
         <v>117</v>
       </c>
       <c r="D104" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="E104" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F104" s="2"/>
+      <c r="E104" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F104" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="105" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="2">
@@ -2846,16 +2997,18 @@
       <c r="B105" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C105" s="21" t="s">
+      <c r="C105" s="17" t="s">
         <v>117</v>
       </c>
       <c r="D105" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="E105" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F105" s="2"/>
+      <c r="E105" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F105" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="106" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="2">
@@ -2864,16 +3017,18 @@
       <c r="B106" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C106" s="21" t="s">
+      <c r="C106" s="17" t="s">
         <v>116</v>
       </c>
       <c r="D106" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="E106" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F106" s="6"/>
+      <c r="E106" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F106" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="107" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="2">
@@ -2882,16 +3037,18 @@
       <c r="B107" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C107" s="21" t="s">
+      <c r="C107" s="17" t="s">
         <v>115</v>
       </c>
       <c r="D107" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="E107" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F107" s="6"/>
+      <c r="E107" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F107" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="108" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="2">
@@ -2900,16 +3057,18 @@
       <c r="B108" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C108" s="21" t="s">
+      <c r="C108" s="17" t="s">
         <v>114</v>
       </c>
       <c r="D108" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="E108" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F108" s="6"/>
+      <c r="E108" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F108" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="109" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="2">
@@ -2918,16 +3077,18 @@
       <c r="B109" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C109" s="21" t="s">
+      <c r="C109" s="17" t="s">
         <v>113</v>
       </c>
       <c r="D109" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="E109" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F109" s="2"/>
+      <c r="E109" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F109" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="110" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="2">
@@ -2936,16 +3097,18 @@
       <c r="B110" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C110" s="21" t="s">
+      <c r="C110" s="17" t="s">
         <v>112</v>
       </c>
       <c r="D110" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="E110" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F110" s="6"/>
+      <c r="E110" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F110" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="111" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="2">
@@ -2954,34 +3117,38 @@
       <c r="B111" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C111" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="D111" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="E111" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F111" s="6"/>
+      <c r="C111" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D111" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E111" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F111" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="112" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="2">
         <v>10</v>
       </c>
-      <c r="B112" s="23" t="s">
+      <c r="B112" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="C112" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="D112" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="E112" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F112" s="6"/>
+      <c r="C112" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D112" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E112" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F112" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="113" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="2">
@@ -2990,59 +3157,61 @@
       <c r="B113" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C113" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="D113" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="E113" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F113" s="6"/>
+      <c r="C113" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D113" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E113" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F113" s="5"/>
     </row>
     <row r="114" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A114" s="10" t="s">
+      <c r="A114" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="B114" s="11"/>
-      <c r="C114" s="11"/>
-      <c r="D114" s="11"/>
-      <c r="E114" s="11"/>
-      <c r="F114" s="12"/>
+      <c r="B114" s="24"/>
+      <c r="C114" s="24"/>
+      <c r="D114" s="24"/>
+      <c r="E114" s="24"/>
+      <c r="F114" s="25"/>
     </row>
     <row r="115" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="2">
         <v>1</v>
       </c>
-      <c r="B115" s="23" t="s">
+      <c r="B115" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="C115" s="19" t="s">
+      <c r="C115" s="15" t="s">
         <v>19</v>
       </c>
       <c r="D115" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="E115" s="24" t="s">
+      <c r="E115" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="F115" s="2"/>
+      <c r="F115" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="116" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="2">
         <v>2</v>
       </c>
-      <c r="B116" s="23" t="s">
+      <c r="B116" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="C116" s="21" t="s">
+      <c r="C116" s="17" t="s">
         <v>111</v>
       </c>
       <c r="D116" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="E116" s="19" t="s">
+      <c r="E116" s="15" t="s">
         <v>19</v>
       </c>
       <c r="F116" s="2"/>
@@ -3054,16 +3223,16 @@
       <c r="B117" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C117" s="21" t="s">
+      <c r="C117" s="17" t="s">
         <v>111</v>
       </c>
       <c r="D117" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="E117" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F117" s="6"/>
+      <c r="E117" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F117" s="5"/>
     </row>
     <row r="118" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="2">
@@ -3072,16 +3241,16 @@
       <c r="B118" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C118" s="21" t="s">
+      <c r="C118" s="17" t="s">
         <v>110</v>
       </c>
       <c r="D118" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="E118" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F118" s="6"/>
+      <c r="E118" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F118" s="5"/>
     </row>
     <row r="119" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="2">
@@ -3090,13 +3259,13 @@
       <c r="B119" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C119" s="21" t="s">
+      <c r="C119" s="17" t="s">
         <v>109</v>
       </c>
       <c r="D119" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="E119" s="19" t="s">
+      <c r="E119" s="15" t="s">
         <v>19</v>
       </c>
       <c r="F119" s="2"/>
@@ -3108,16 +3277,16 @@
       <c r="B120" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C120" s="21" t="s">
+      <c r="C120" s="17" t="s">
         <v>108</v>
       </c>
       <c r="D120" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="E120" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F120" s="6"/>
+      <c r="E120" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F120" s="5"/>
     </row>
     <row r="121" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="2">
@@ -3126,13 +3295,13 @@
       <c r="B121" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C121" s="21" t="s">
+      <c r="C121" s="17" t="s">
         <v>107</v>
       </c>
       <c r="D121" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="E121" s="19" t="s">
+      <c r="E121" s="15" t="s">
         <v>19</v>
       </c>
       <c r="F121" s="2"/>
@@ -3144,16 +3313,16 @@
       <c r="B122" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C122" s="21" t="s">
+      <c r="C122" s="17" t="s">
         <v>106</v>
       </c>
       <c r="D122" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="E122" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F122" s="6"/>
+      <c r="E122" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F122" s="5"/>
     </row>
     <row r="123" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="2">
@@ -3162,16 +3331,16 @@
       <c r="B123" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C123" s="21" t="s">
+      <c r="C123" s="17" t="s">
         <v>105</v>
       </c>
       <c r="D123" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="E123" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F123" s="6"/>
+      <c r="E123" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F123" s="5"/>
     </row>
     <row r="124" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="2">
@@ -3180,13 +3349,13 @@
       <c r="B124" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C124" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="D124" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="E124" s="19" t="s">
+      <c r="C124" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D124" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E124" s="15" t="s">
         <v>19</v>
       </c>
       <c r="F124" s="2"/>
@@ -3195,19 +3364,19 @@
       <c r="A125" s="2">
         <v>11</v>
       </c>
-      <c r="B125" s="23" t="s">
+      <c r="B125" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="C125" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="D125" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="E125" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F125" s="6"/>
+      <c r="C125" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D125" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E125" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F125" s="5"/>
     </row>
     <row r="126" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="2">
@@ -3216,62 +3385,66 @@
       <c r="B126" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C126" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="D126" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="E126" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F126" s="6"/>
+      <c r="C126" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D126" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E126" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F126" s="5"/>
     </row>
     <row r="127" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A127" s="10" t="s">
+      <c r="A127" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="B127" s="11"/>
-      <c r="C127" s="11"/>
-      <c r="D127" s="11"/>
-      <c r="E127" s="11"/>
-      <c r="F127" s="12"/>
+      <c r="B127" s="24"/>
+      <c r="C127" s="24"/>
+      <c r="D127" s="24"/>
+      <c r="E127" s="24"/>
+      <c r="F127" s="25"/>
     </row>
     <row r="128" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="2">
         <v>1</v>
       </c>
-      <c r="B128" s="23" t="s">
-        <v>92</v>
-      </c>
-      <c r="C128" s="19" t="s">
+      <c r="B128" s="27" t="s">
+        <v>153</v>
+      </c>
+      <c r="C128" s="15" t="s">
         <v>19</v>
       </c>
       <c r="D128" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E128" s="24" t="s">
+      <c r="E128" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="F128" s="2"/>
+      <c r="F128" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="129" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="2">
         <v>2</v>
       </c>
-      <c r="B129" s="23" t="s">
-        <v>93</v>
-      </c>
-      <c r="C129" s="21" t="s">
+      <c r="B129" s="27" t="s">
+        <v>154</v>
+      </c>
+      <c r="C129" s="17" t="s">
         <v>104</v>
       </c>
       <c r="D129" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E129" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F129" s="6"/>
+      <c r="E129" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F129" s="12" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="130" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="2">
@@ -3280,16 +3453,16 @@
       <c r="B130" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C130" s="21" t="s">
+      <c r="C130" s="17" t="s">
         <v>104</v>
       </c>
       <c r="D130" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E130" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F130" s="6"/>
+      <c r="E130" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F130" s="5"/>
     </row>
     <row r="131" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="2">
@@ -3298,16 +3471,16 @@
       <c r="B131" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C131" s="21" t="s">
+      <c r="C131" s="17" t="s">
         <v>103</v>
       </c>
       <c r="D131" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E131" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F131" s="6"/>
+      <c r="E131" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F131" s="5"/>
     </row>
     <row r="132" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="2">
@@ -3316,16 +3489,16 @@
       <c r="B132" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C132" s="21" t="s">
+      <c r="C132" s="17" t="s">
         <v>102</v>
       </c>
       <c r="D132" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E132" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F132" s="6"/>
+      <c r="E132" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F132" s="5"/>
     </row>
     <row r="133" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="2">
@@ -3334,16 +3507,16 @@
       <c r="B133" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C133" s="21" t="s">
+      <c r="C133" s="17" t="s">
         <v>101</v>
       </c>
       <c r="D133" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E133" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F133" s="6"/>
+      <c r="E133" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F133" s="5"/>
     </row>
     <row r="134" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="2">
@@ -3352,16 +3525,16 @@
       <c r="B134" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C134" s="21" t="s">
+      <c r="C134" s="17" t="s">
         <v>100</v>
       </c>
       <c r="D134" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E134" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F134" s="6"/>
+      <c r="E134" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F134" s="5"/>
     </row>
     <row r="135" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="2">
@@ -3370,16 +3543,16 @@
       <c r="B135" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C135" s="21" t="s">
+      <c r="C135" s="17" t="s">
         <v>99</v>
       </c>
       <c r="D135" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E135" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F135" s="6"/>
+      <c r="E135" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F135" s="5"/>
     </row>
     <row r="136" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="2">
@@ -3388,16 +3561,16 @@
       <c r="B136" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C136" s="21" t="s">
+      <c r="C136" s="17" t="s">
         <v>98</v>
       </c>
       <c r="D136" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E136" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F136" s="6"/>
+      <c r="E136" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F136" s="5"/>
     </row>
     <row r="137" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="2">
@@ -3406,31 +3579,31 @@
       <c r="B137" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C137" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="D137" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="E137" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F137" s="6"/>
+      <c r="C137" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D137" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E137" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F137" s="5"/>
     </row>
     <row r="138" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="2">
         <v>11</v>
       </c>
-      <c r="B138" s="23" t="s">
+      <c r="B138" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="C138" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="D138" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="E138" s="19" t="s">
+      <c r="C138" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D138" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E138" s="15" t="s">
         <v>19</v>
       </c>
       <c r="F138" s="2"/>
@@ -3442,16 +3615,16 @@
       <c r="B139" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C139" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="D139" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="E139" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F139" s="6"/>
+      <c r="C139" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D139" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E139" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F139" s="5"/>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B140"/>
@@ -3551,11 +3724,6 @@
   </sheetData>
   <autoFilter ref="D3:D204" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="13">
-    <mergeCell ref="A127:F127"/>
-    <mergeCell ref="A78:F78"/>
-    <mergeCell ref="A90:F90"/>
-    <mergeCell ref="A102:F102"/>
-    <mergeCell ref="A114:F114"/>
     <mergeCell ref="A28:F28"/>
     <mergeCell ref="A41:F41"/>
     <mergeCell ref="A53:F53"/>
@@ -3564,6 +3732,11 @@
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A4:F4"/>
     <mergeCell ref="A15:F15"/>
+    <mergeCell ref="A127:F127"/>
+    <mergeCell ref="A78:F78"/>
+    <mergeCell ref="A90:F90"/>
+    <mergeCell ref="A102:F102"/>
+    <mergeCell ref="A114:F114"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="92" fitToHeight="0" orientation="landscape"/>

</xml_diff>